<commit_message>
state machine diagnostics and Occupgrid
</commit_message>
<xml_diff>
--- a/AVC_Docs/AVC_CmdAndTlmAndTest_v2.xlsx
+++ b/AVC_Docs/AVC_CmdAndTlmAndTest_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="13430" yWindow="0" windowWidth="15360" windowHeight="11020" tabRatio="828" activeTab="1"/>
+    <workbookView xWindow="10380" yWindow="0" windowWidth="15360" windowHeight="11025" tabRatio="828" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Rpi to Iop Cmds" sheetId="1" r:id="rId1"/>
@@ -383,18 +383,6 @@
     <t>Ascii 'B'  (66)</t>
   </si>
   <si>
-    <t>Object Type: 
-'N' - (78) none
-'B' - (66) barrels
-'H' - (72) hoop
-'R' - (82) ramp
-'P'- (80) pedestrian only
-'S'- (83) stopsign only
-'Q' -(81) both pedestrian and stopsign
-'C' - (67) horizontal crosswalk
-'E' - (69) end-of-course horizontal strip</t>
-  </si>
-  <si>
     <t>Message value
 2 bytes</t>
   </si>
@@ -998,6 +986,19 @@
   </si>
   <si>
     <t>Current distance of Sensor 3</t>
+  </si>
+  <si>
+    <t>Object Type: 
+'N' - (78) none
+'B' - (66) barrels
+'H' - (72) hoop
+'R' - (82) ramp
+'P'- (80) pedestrian only
+'S'- (83) stopsign only
+'C' - (67) crosswalk
+'Q' -(81) both pedestrian and stopsign
+'C' - (67) horizontal crosswalk
+'E' - (69) end-of-course horizontal strip</t>
   </si>
 </sst>
 </file>
@@ -1931,45 +1932,45 @@
       <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="47.26953125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="63" style="4" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" style="4"/>
-    <col min="9" max="9" width="11.81640625" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="4"/>
+    <col min="8" max="8" width="9.140625" style="4"/>
+    <col min="9" max="9" width="11.85546875" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -1980,19 +1981,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="F3" s="17">
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -2015,7 +2016,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -2026,7 +2027,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -2038,7 +2039,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -2049,7 +2050,7 @@
         <v>84</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>6</v>
@@ -2061,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2072,7 +2073,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>12</v>
@@ -2084,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2095,7 +2096,7 @@
         <v>88</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>14</v>
@@ -2107,7 +2108,7 @@
         <v>16</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2118,7 +2119,7 @@
         <v>89</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>14</v>
@@ -2130,7 +2131,7 @@
         <v>19</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2141,7 +2142,7 @@
         <v>74</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>75</v>
@@ -2153,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -2164,7 +2165,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>31</v>
@@ -2176,7 +2177,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2187,7 +2188,7 @@
         <v>81</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D12" s="4">
         <v>0</v>
@@ -2199,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2210,10 +2211,10 @@
         <v>51</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E13" s="17">
         <v>0</v>
@@ -2222,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -2233,19 +2234,19 @@
         <v>72</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="F14" s="17">
         <v>0</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2256,10 +2257,10 @@
         <v>95</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E15" s="17">
         <v>0</v>
@@ -2268,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -2279,7 +2280,7 @@
         <v>86</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>87</v>
@@ -2291,43 +2292,43 @@
         <v>0</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D17" s="17" t="s">
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E17" s="4">
-        <v>0</v>
-      </c>
-      <c r="F17" s="17">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="43" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:7" s="43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="43" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" s="43" t="s">
         <v>202</v>
-      </c>
-      <c r="B18" s="43" t="s">
-        <v>203</v>
       </c>
       <c r="D18" s="44"/>
       <c r="F18" s="44"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>57</v>
       </c>
@@ -2342,7 +2343,7 @@
       </c>
       <c r="F19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>56</v>
       </c>
@@ -2357,62 +2358,62 @@
       </c>
       <c r="F20" s="17"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="D21" s="17"/>
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="176.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>44</v>
       </c>
@@ -2420,7 +2421,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>45</v>
       </c>
@@ -2428,7 +2429,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>46</v>
       </c>
@@ -2436,7 +2437,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
     </row>
   </sheetData>
@@ -2449,33 +2450,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.81640625" customWidth="1"/>
-    <col min="2" max="2" width="38.81640625" customWidth="1"/>
-    <col min="3" max="3" width="7.1796875" style="31" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" style="31" customWidth="1"/>
     <col min="4" max="4" width="10" style="31" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" style="31" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" style="31" customWidth="1"/>
-    <col min="7" max="7" width="8.1796875" style="31" customWidth="1"/>
-    <col min="8" max="8" width="10.7265625" style="31" customWidth="1"/>
-    <col min="9" max="9" width="3.81640625" style="33" customWidth="1"/>
-    <col min="10" max="10" width="74.7265625" style="35" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="31" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="31" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="31" customWidth="1"/>
+    <col min="9" max="9" width="3.85546875" style="33" customWidth="1"/>
+    <col min="10" max="10" width="74.7109375" style="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>36</v>
@@ -2484,7 +2485,7 @@
         <v>33</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>59</v>
@@ -2494,15 +2495,15 @@
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="34" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2" s="36">
         <v>1</v>
@@ -2518,7 +2519,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H2" s="39">
         <v>0</v>
@@ -2526,7 +2527,7 @@
       <c r="I2" s="40"/>
       <c r="J2" s="41"/>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>4</v>
       </c>
@@ -2548,14 +2549,14 @@
         <v>4</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H3" s="25">
         <f t="shared" ref="H3:H21" si="0">H2+1</f>
         <v>1</v>
       </c>
       <c r="J3" s="35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2587,7 +2588,7 @@
         <v>2</v>
       </c>
       <c r="J4" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2619,7 +2620,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -2651,7 +2652,7 @@
         <v>4</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="87" x14ac:dyDescent="0.35">
@@ -2659,7 +2660,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C7" s="17">
         <v>1</v>
@@ -2683,10 +2684,10 @@
         <v>5</v>
       </c>
       <c r="J7" s="34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="29.15" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>25</v>
       </c>
@@ -2715,10 +2716,10 @@
         <v>6</v>
       </c>
       <c r="J8" s="34" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="101.45" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>64</v>
       </c>
@@ -2747,12 +2748,12 @@
         <v>7</v>
       </c>
       <c r="J9" s="34" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>52</v>
@@ -2779,12 +2780,12 @@
         <v>8</v>
       </c>
       <c r="J10" s="35" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>52</v>
@@ -2811,12 +2812,12 @@
         <v>9</v>
       </c>
       <c r="J11" s="35" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>52</v>
@@ -2843,12 +2844,12 @@
         <v>10</v>
       </c>
       <c r="J12" s="35" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A13" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>52</v>
@@ -2875,10 +2876,10 @@
         <v>11</v>
       </c>
       <c r="J13" s="35" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
         <v>41</v>
       </c>
@@ -2907,15 +2908,15 @@
         <v>12</v>
       </c>
       <c r="J14" s="34" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="57.95" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C15" s="17">
         <v>1</v>
@@ -2939,12 +2940,12 @@
         <v>13</v>
       </c>
       <c r="J15" s="34" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="57.95" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="17">
@@ -2969,10 +2970,10 @@
         <v>14</v>
       </c>
       <c r="J16" s="34" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
         <v>104</v>
       </c>
@@ -3001,10 +3002,10 @@
         <v>15</v>
       </c>
       <c r="J17" s="35" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
         <v>82</v>
       </c>
@@ -3033,10 +3034,10 @@
         <v>16</v>
       </c>
       <c r="J18" s="35" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
         <v>83</v>
       </c>
@@ -3065,10 +3066,10 @@
         <v>17</v>
       </c>
       <c r="J19" s="35" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
         <v>61</v>
       </c>
@@ -3097,10 +3098,10 @@
         <v>18</v>
       </c>
       <c r="J20" s="34" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>63</v>
       </c>
@@ -3129,10 +3130,10 @@
         <v>19</v>
       </c>
       <c r="J21" s="34" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>78</v>
       </c>
@@ -3161,10 +3162,10 @@
         <v>20</v>
       </c>
       <c r="J22" s="34" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>92</v>
       </c>
@@ -3193,15 +3194,15 @@
         <v>21</v>
       </c>
       <c r="J23" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="C24" s="17">
         <v>1</v>
@@ -3225,7 +3226,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>65</v>
       </c>
@@ -3252,7 +3253,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>65</v>
       </c>
@@ -3279,7 +3280,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="16" t="s">
         <v>34</v>
@@ -3294,7 +3295,7 @@
       <c r="G27" s="27"/>
       <c r="H27" s="25"/>
     </row>
-    <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="B28" s="13"/>
       <c r="C28" s="28"/>
@@ -3318,26 +3319,26 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.81640625" customWidth="1"/>
-    <col min="2" max="2" width="38.81640625" customWidth="1"/>
-    <col min="3" max="3" width="7.1796875" style="31" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" style="31" customWidth="1"/>
     <col min="4" max="4" width="10" style="31" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" style="31" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" style="31" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="31" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="31" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>36</v>
@@ -3346,18 +3347,18 @@
         <v>33</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G1" s="24" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C2" s="36">
         <v>1</v>
@@ -3376,7 +3377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>4</v>
       </c>
@@ -3402,12 +3403,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="C4" s="17">
         <v>1</v>
@@ -3428,12 +3429,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C5" s="17">
         <v>1</v>
@@ -3454,12 +3455,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6" s="17">
         <v>1</v>
@@ -3480,12 +3481,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7" s="17">
         <v>1</v>
@@ -3506,12 +3507,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C8" s="17">
         <v>1</v>
@@ -3532,12 +3533,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C9" s="17">
         <v>1</v>
@@ -3558,12 +3559,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C10" s="17">
         <v>1</v>
@@ -3584,12 +3585,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C11" s="17">
         <v>1</v>
@@ -3610,12 +3611,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C12" s="17">
         <v>1</v>
@@ -3636,7 +3637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="16" t="s">
         <v>34</v>
@@ -3672,20 +3673,20 @@
       <selection activeCell="A2" sqref="A2:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.453125" style="60" customWidth="1"/>
-    <col min="2" max="2" width="31.54296875" style="72" customWidth="1"/>
-    <col min="3" max="3" width="7.1796875" style="60" customWidth="1"/>
-    <col min="4" max="4" width="2.81640625" style="60" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" style="60" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" style="60" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="72" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" style="60" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" style="60" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="60" customWidth="1"/>
     <col min="6" max="8" width="13" style="60" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="60"/>
+    <col min="9" max="16384" width="9.140625" style="60"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="57" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="59" t="s">
@@ -3695,19 +3696,19 @@
       <c r="F1" s="45"/>
       <c r="G1" s="45"/>
     </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" s="63"/>
       <c r="E2" s="45"/>
       <c r="F2" s="45"/>
       <c r="G2" s="45"/>
     </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>96</v>
       </c>
@@ -3718,7 +3719,7 @@
       <c r="D3" s="65"/>
       <c r="H3" s="49"/>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>97</v>
       </c>
@@ -3731,12 +3732,12 @@
       <c r="G4" s="49"/>
       <c r="H4" s="49"/>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="C5" s="64"/>
       <c r="D5" s="65"/>
@@ -3757,7 +3758,7 @@
       <c r="G6" s="45"/>
       <c r="H6" s="49"/>
     </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>99</v>
       </c>
@@ -3767,7 +3768,7 @@
       <c r="C7" s="64"/>
       <c r="D7" s="65"/>
       <c r="E7" s="66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F7" s="49"/>
       <c r="G7" s="49"/>
@@ -3783,7 +3784,7 @@
       <c r="C8" s="64"/>
       <c r="D8" s="65"/>
       <c r="E8" s="67" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" s="49"/>
       <c r="G8" s="49"/>
@@ -3805,10 +3806,10 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="69" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="70" t="s">
         <v>122</v>
-      </c>
-      <c r="B10" s="70" t="s">
-        <v>123</v>
       </c>
       <c r="C10" s="71"/>
       <c r="D10" s="65"/>
@@ -3827,23 +3828,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.453125" style="46" customWidth="1"/>
-    <col min="2" max="2" width="35.7265625" style="46" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" style="46" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" style="46" customWidth="1"/>
     <col min="3" max="3" width="12" style="46" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="46"/>
+    <col min="4" max="4" width="9.140625" style="46"/>
     <col min="5" max="5" width="13" style="46" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="46"/>
+    <col min="6" max="16384" width="9.140625" style="46"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="11" t="s">
@@ -3855,12 +3856,12 @@
       <c r="G1" s="45"/>
       <c r="H1" s="45"/>
     </row>
-    <row r="2" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>106</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>113</v>
+        <v>270</v>
       </c>
       <c r="C2" s="25">
         <v>2</v>
@@ -3895,13 +3896,13 @@
       </c>
       <c r="D4" s="48"/>
       <c r="E4" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="51"/>
       <c r="H4" s="52"/>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="4" t="s">
         <v>104</v>
@@ -3934,13 +3935,13 @@
       </c>
       <c r="D6" s="48"/>
       <c r="E6" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="13" t="s">
         <v>116</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>117</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>104</v>
@@ -3959,57 +3960,57 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.453125" style="80" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" style="73" customWidth="1"/>
-    <col min="3" max="3" width="45.81640625" style="73" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" style="73" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" style="80" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="73" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" style="73" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="73" customWidth="1"/>
     <col min="5" max="7" width="10" style="74" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" style="73"/>
-    <col min="9" max="9" width="30.1796875" style="73" customWidth="1"/>
-    <col min="10" max="11" width="44.26953125" style="73" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="73"/>
+    <col min="8" max="8" width="9.140625" style="73"/>
+    <col min="9" max="9" width="30.140625" style="73" customWidth="1"/>
+    <col min="10" max="11" width="44.28515625" style="73" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="73"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="45" customFormat="1" ht="29.15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="45" customFormat="1" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="75" t="s">
+      <c r="G1" s="76" t="s">
         <v>142</v>
-      </c>
-      <c r="F1" s="75" t="s">
-        <v>141</v>
-      </c>
-      <c r="G1" s="76" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="49" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>215</v>
-      </c>
       <c r="E2" s="56" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F2" s="56">
         <v>0</v>
@@ -4020,45 +4021,45 @@
     </row>
     <row r="3" spans="1:10" s="49" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="56" t="s">
         <v>217</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="F3" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="F3" s="56" t="s">
-        <v>219</v>
-      </c>
       <c r="G3" s="77">
         <v>0</v>
       </c>
       <c r="J3" s="49" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="49" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="56" t="s">
         <v>225</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="E4" s="56" t="s">
-        <v>226</v>
       </c>
       <c r="F4" s="56">
         <v>0</v>
@@ -4069,19 +4070,19 @@
     </row>
     <row r="5" spans="1:10" s="49" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>228</v>
-      </c>
       <c r="E5" s="56" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F5" s="56">
         <v>0</v>
@@ -4090,18 +4091,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="49" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>258</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>259</v>
       </c>
       <c r="E6" s="56">
         <v>0</v>
@@ -4115,20 +4116,20 @@
     </row>
     <row r="7" spans="1:10" s="49" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="E7" s="56" t="s">
         <v>236</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="E7" s="56" t="s">
-        <v>237</v>
-      </c>
       <c r="F7" s="56">
         <v>0</v>
       </c>
@@ -4136,19 +4137,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>263</v>
-      </c>
       <c r="E8" s="56">
         <v>0</v>
       </c>
@@ -4159,35 +4160,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="49" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" s="49" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F9" s="56" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G9" s="77">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="49" customFormat="1" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" s="49" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -4205,18 +4206,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="49" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" s="49" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E11" s="56">
         <v>0</v>
@@ -4228,18 +4229,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="49" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" s="49" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E12" s="56" t="s">
         <v>12</v>
@@ -4251,18 +4252,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="49" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" s="49" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E13" s="56" t="s">
         <v>14</v>
@@ -4274,18 +4275,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="49" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" s="49" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>89</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E14" s="56" t="s">
         <v>14</v>
@@ -4297,18 +4298,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="49" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" s="49" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>73</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E15" s="56" t="s">
         <v>75</v>
@@ -4320,18 +4321,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="49" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" s="49" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E16" s="56" t="s">
         <v>31</v>
@@ -4345,18 +4346,18 @@
       <c r="I16" s="73"/>
       <c r="J16" s="73"/>
     </row>
-    <row r="17" spans="1:10" s="49" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" s="49" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E17" s="56">
         <v>0</v>
@@ -4370,21 +4371,21 @@
       <c r="I17" s="73"/>
       <c r="J17" s="73"/>
     </row>
-    <row r="18" spans="1:10" s="49" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" s="49" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>70</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E18" s="56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F18" s="56">
         <v>0</v>
@@ -4395,24 +4396,24 @@
       <c r="I18" s="73"/>
       <c r="J18" s="73"/>
     </row>
-    <row r="19" spans="1:10" s="49" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" s="49" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>71</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E19" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="F19" s="56" t="s">
         <v>144</v>
-      </c>
-      <c r="F19" s="56" t="s">
-        <v>145</v>
       </c>
       <c r="G19" s="77">
         <v>0</v>
@@ -4420,21 +4421,21 @@
       <c r="I19" s="73"/>
       <c r="J19" s="73"/>
     </row>
-    <row r="20" spans="1:10" s="49" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" s="49" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>94</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>95</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E20" s="56" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F20" s="56">
         <v>0</v>
@@ -4445,18 +4446,18 @@
       <c r="I20" s="73"/>
       <c r="J20" s="73"/>
     </row>
-    <row r="21" spans="1:10" s="49" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" s="49" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>85</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>86</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E21" s="56" t="s">
         <v>87</v>
@@ -4470,21 +4471,21 @@
       <c r="I21" s="73"/>
       <c r="J21" s="73"/>
     </row>
-    <row r="22" spans="1:10" s="49" customFormat="1" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" s="49" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="C22" s="13" t="s">
+      <c r="D22" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="E22" s="78" t="s">
         <v>137</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="E22" s="78" t="s">
-        <v>138</v>
       </c>
       <c r="F22" s="78">
         <v>0</v>
@@ -4509,22 +4510,22 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.1796875" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>36</v>
@@ -4533,7 +4534,7 @@
         <v>33</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>59</v>
@@ -4544,10 +4545,10 @@
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2" s="36">
         <v>1</v>
@@ -4563,13 +4564,13 @@
         <v>0</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H2" s="39">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="4"/>
       <c r="C3" s="17"/>
@@ -4579,7 +4580,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="25"/>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
       <c r="B4" s="4"/>
       <c r="C4" s="17"/>
@@ -4589,7 +4590,7 @@
       <c r="G4" s="19"/>
       <c r="H4" s="25"/>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="4"/>
       <c r="C5" s="17"/>
@@ -4599,7 +4600,7 @@
       <c r="G5" s="19"/>
       <c r="H5" s="25"/>
     </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="4"/>
       <c r="C6" s="17"/>
@@ -4609,7 +4610,7 @@
       <c r="G6" s="19"/>
       <c r="H6" s="25"/>
     </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="4"/>
       <c r="C7" s="17"/>
@@ -4633,21 +4634,21 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.81640625" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
     <col min="2" max="2" width="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>36</v>
@@ -4656,7 +4657,7 @@
         <v>33</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G1" s="27" t="s">
         <v>59</v>
@@ -4665,12 +4666,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C2" s="17">
         <v>1</v>
@@ -4686,13 +4687,13 @@
         <v>0</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H2" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -4714,19 +4715,19 @@
         <v>4</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H3" s="17">
         <f t="shared" ref="H3:H9" si="0">H2+1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>251</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>252</v>
       </c>
       <c r="C4" s="17">
         <v>1</v>
@@ -4749,10 +4750,10 @@
     </row>
     <row r="5" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C5" s="17">
         <v>1</v>
@@ -4779,10 +4780,10 @@
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C6" s="17">
         <v>1</v>
@@ -4809,10 +4810,10 @@
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C7" s="17">
         <v>1</v>
@@ -4839,10 +4840,10 @@
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="17">
         <v>1</v>
@@ -4869,10 +4870,10 @@
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C9" s="17">
         <v>1</v>
@@ -4897,7 +4898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="17"/>
@@ -4921,21 +4922,21 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.81640625" customWidth="1"/>
-    <col min="2" max="2" width="27.26953125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>36</v>
@@ -4944,7 +4945,7 @@
         <v>33</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>59</v>
@@ -4953,12 +4954,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C2" s="36">
         <v>1</v>
@@ -4974,13 +4975,13 @@
         <v>0</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H2" s="39">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>4</v>
       </c>
@@ -5002,19 +5003,19 @@
         <v>4</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H3" s="25">
         <f t="shared" ref="H3:H12" si="0">H2+1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="C4" s="17">
         <v>1</v>
@@ -5040,10 +5041,10 @@
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C5" s="17">
         <v>1</v>
@@ -5069,10 +5070,10 @@
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6" s="17">
         <v>1</v>
@@ -5098,10 +5099,10 @@
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7" s="17">
         <v>1</v>
@@ -5127,10 +5128,10 @@
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C8" s="17">
         <v>1</v>
@@ -5156,10 +5157,10 @@
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C9" s="17">
         <v>1</v>
@@ -5185,10 +5186,10 @@
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C10" s="17">
         <v>1</v>
@@ -5214,10 +5215,10 @@
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C11" s="17">
         <v>1</v>
@@ -5243,10 +5244,10 @@
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C12" s="17">
         <v>1</v>
@@ -5270,7 +5271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="16" t="s">
         <v>34</v>
@@ -5285,7 +5286,7 @@
       <c r="G13" s="27"/>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
       <c r="C14" s="28"/>

</xml_diff>

<commit_message>
Added IOP command diagnostics and command re-syncing
</commit_message>
<xml_diff>
--- a/AVC_Docs/AVC_CmdAndTlmAndTest_v2.xlsx
+++ b/AVC_Docs/AVC_CmdAndTlmAndTest_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10380" yWindow="0" windowWidth="15360" windowHeight="11025" tabRatio="828" activeTab="4"/>
+    <workbookView xWindow="10380" yWindow="0" windowWidth="15360" windowHeight="11020" tabRatio="828"/>
   </bookViews>
   <sheets>
     <sheet name="Rpi to Iop Cmds" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="276">
   <si>
     <t>Notes</t>
   </si>
@@ -146,9 +146,6 @@
     <t>convert all IR sensor values to real world values</t>
   </si>
   <si>
-    <t>Current angle  front looking IR sensors</t>
-  </si>
-  <si>
     <t>milliVolts</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
   </si>
   <si>
     <t>Cumulative distance from when put into Normal mode</t>
-  </si>
-  <si>
-    <t>spares</t>
   </si>
   <si>
     <t>milliseconds (32 bits total)</t>
@@ -344,9 +338,6 @@
     <t>Look for Ramp</t>
   </si>
   <si>
-    <t>Look for horizontal end-of-course strip (color?)</t>
-  </si>
-  <si>
     <t>Look for horizontal crosswalk strip (color?)</t>
   </si>
   <si>
@@ -381,10 +372,6 @@
   </si>
   <si>
     <t>Ascii 'B'  (66)</t>
-  </si>
-  <si>
-    <t>Message value
-2 bytes</t>
   </si>
   <si>
     <t>Object Found</t>
@@ -599,12 +586,6 @@
    - verify all the angles are within this range</t>
   </si>
   <si>
-    <t>1 - send command to use the 100-550 sensor.  Change range between 200 and 400 cm.
-    - Verify the reported range is in this range and the telemetry reflects this sensor
-2 - send command to use the 20-150 sensor.  Change range between40 and 100 cm.
-    - Verify the reported range is in this range and the telemetry reflects this sensor</t>
-  </si>
-  <si>
     <t>Done above</t>
   </si>
   <si>
@@ -968,12 +949,6 @@
   </si>
   <si>
     <t>Current distance of Sensor 1</t>
-  </si>
-  <si>
-    <t>0.01 degress resolution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spare </t>
   </si>
   <si>
     <t>cm per second</t>
@@ -999,6 +974,46 @@
 'Q' -(81) both pedestrian and stopsign
 'C' - (67) horizontal crosswalk
 'E' - (69) end-of-course horizontal strip</t>
+  </si>
+  <si>
+    <t>Always 0x44454144 (ascii 'DEAD')</t>
+  </si>
+  <si>
+    <t>Current angle  of the scanner</t>
+  </si>
+  <si>
+    <t>spares - left wheel encoder count</t>
+  </si>
+  <si>
+    <t>spares -  right wheel encoder count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Num of rejected Cmds.  For each invalid command increment this value.  </t>
+  </si>
+  <si>
+    <t>Number of rejected commands</t>
+  </si>
+  <si>
+    <t>Last rejected command reason</t>
+  </si>
+  <si>
+    <t>CMD Header (always 0x5454)</t>
+  </si>
+  <si>
+    <t>CMD Header (always 0x5656)</t>
+  </si>
+  <si>
+    <t>Command ID</t>
+  </si>
+  <si>
+    <t>Look for horizontal end-of-course strip</t>
+  </si>
+  <si>
+    <t>1 - Bad header
+2 - Unrecognized command
+3 - Incorrect mode
+4 - Out of limits
+5 - Unknown (should never occur)</t>
   </si>
 </sst>
 </file>
@@ -1216,10 +1231,25 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -1231,13 +1261,24 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1249,10 +1290,8 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1264,10 +1303,8 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1279,8 +1316,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1292,32 +1331,41 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -1325,58 +1373,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1445,7 +1446,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1460,7 +1461,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1494,108 +1495,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1610,7 +1581,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1624,6 +1595,36 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1928,49 +1929,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="32.54296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="47.26953125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" style="4" customWidth="1"/>
     <col min="7" max="7" width="63" style="4" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="4"/>
-    <col min="9" max="9" width="11.85546875" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="8" max="8" width="9.1796875" style="4"/>
+    <col min="9" max="9" width="11.81640625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -1981,19 +1982,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F3" s="17">
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -2004,7 +2005,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
@@ -2016,18 +2017,18 @@
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -2039,7 +2040,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -2047,10 +2048,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>6</v>
@@ -2062,18 +2063,18 @@
         <v>0</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>12</v>
@@ -2085,7 +2086,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2093,10 +2094,10 @@
         <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>14</v>
@@ -2108,7 +2109,7 @@
         <v>16</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2116,10 +2117,10 @@
         <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>14</v>
@@ -2131,30 +2132,30 @@
         <v>19</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="F10" s="17">
         <v>0</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -2162,10 +2163,10 @@
         <v>30</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>31</v>
@@ -2177,18 +2178,18 @@
         <v>0</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D12" s="4">
         <v>0</v>
@@ -2200,21 +2201,21 @@
         <v>0</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E13" s="17">
         <v>0</v>
@@ -2223,44 +2224,44 @@
         <v>0</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F14" s="17">
         <v>0</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E15" s="17">
         <v>0</v>
@@ -2269,22 +2270,22 @@
         <v>0</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="E16" s="17">
         <v>0</v>
       </c>
@@ -2292,152 +2293,158 @@
         <v>0</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E17" s="4">
-        <v>0</v>
-      </c>
-      <c r="F17" s="17">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="43" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="43" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D18" s="44"/>
       <c r="F18" s="44"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="10" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="73" t="s">
+        <v>271</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="E19" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>56</v>
+      <c r="B20" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="D21" s="17"/>
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="176.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="B33" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="B34" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B41" s="3"/>
     </row>
   </sheetData>
@@ -2450,33 +2457,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="44.81640625" customWidth="1"/>
+    <col min="2" max="2" width="38.81640625" customWidth="1"/>
+    <col min="3" max="3" width="7.1796875" style="31" customWidth="1"/>
     <col min="4" max="4" width="10" style="31" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="31" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="31" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="31" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="31" customWidth="1"/>
-    <col min="9" max="9" width="3.85546875" style="33" customWidth="1"/>
-    <col min="10" max="10" width="74.7109375" style="35" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" style="31" customWidth="1"/>
+    <col min="6" max="6" width="7.7265625" style="31" customWidth="1"/>
+    <col min="7" max="7" width="8.1796875" style="31" customWidth="1"/>
+    <col min="8" max="8" width="10.7265625" style="31" customWidth="1"/>
+    <col min="9" max="9" width="3.81640625" style="33" customWidth="1"/>
+    <col min="10" max="10" width="74.7265625" style="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>36</v>
@@ -2485,25 +2492,25 @@
         <v>33</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I1" s="32"/>
       <c r="J1" s="34" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="37" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>189</v>
+        <v>264</v>
       </c>
       <c r="C2" s="36">
         <v>1</v>
@@ -2519,7 +2526,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H2" s="39">
         <v>0</v>
@@ -2527,12 +2534,12 @@
       <c r="I2" s="40"/>
       <c r="J2" s="41"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="17">
         <v>1</v>
@@ -2549,14 +2556,14 @@
         <v>4</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H3" s="25">
         <f t="shared" ref="H3:H21" si="0">H2+1</f>
         <v>1</v>
       </c>
       <c r="J3" s="35" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -2588,12 +2595,12 @@
         <v>2</v>
       </c>
       <c r="J4" s="34" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
@@ -2620,15 +2627,15 @@
         <v>3</v>
       </c>
       <c r="J5" s="35" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="17">
         <v>1</v>
@@ -2652,7 +2659,7 @@
         <v>4</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="87" x14ac:dyDescent="0.35">
@@ -2660,7 +2667,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C7" s="17">
         <v>1</v>
@@ -2684,10 +2691,10 @@
         <v>5</v>
       </c>
       <c r="J7" s="34" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="29.1" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="29.15" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>25</v>
       </c>
@@ -2716,15 +2723,15 @@
         <v>6</v>
       </c>
       <c r="J8" s="34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="101.45" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="17">
         <v>1</v>
@@ -2748,15 +2755,15 @@
         <v>7</v>
       </c>
       <c r="J9" s="34" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="17">
         <v>1</v>
@@ -2780,15 +2787,15 @@
         <v>8</v>
       </c>
       <c r="J10" s="35" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="17">
         <v>1</v>
@@ -2812,15 +2819,15 @@
         <v>9</v>
       </c>
       <c r="J11" s="35" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="17">
         <v>1</v>
@@ -2844,15 +2851,15 @@
         <v>10</v>
       </c>
       <c r="J12" s="35" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="20" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="17">
         <v>1</v>
@@ -2876,15 +2883,15 @@
         <v>11</v>
       </c>
       <c r="J13" s="35" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="29.1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="29.15" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C14" s="17">
         <v>1</v>
@@ -2908,15 +2915,15 @@
         <v>12</v>
       </c>
       <c r="J14" s="34" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="57.95" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
-        <v>39</v>
+        <v>265</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>264</v>
+        <v>37</v>
       </c>
       <c r="C15" s="17">
         <v>1</v>
@@ -2940,14 +2947,16 @@
         <v>13</v>
       </c>
       <c r="J15" s="34" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="57.95" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
-        <v>265</v>
-      </c>
-      <c r="B16" s="4"/>
+        <v>268</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>269</v>
+      </c>
       <c r="C16" s="17">
         <v>1</v>
       </c>
@@ -2969,16 +2978,14 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="J16" s="34" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="J16" s="34"/>
+    </row>
+    <row r="17" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
-        <v>104</v>
+        <v>270</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>52</v>
+        <v>275</v>
       </c>
       <c r="C17" s="17">
         <v>1</v>
@@ -3002,15 +3009,15 @@
         <v>15</v>
       </c>
       <c r="J17" s="35" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="17">
         <v>1</v>
@@ -3034,15 +3041,15 @@
         <v>16</v>
       </c>
       <c r="J18" s="35" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="17">
         <v>1</v>
@@ -3066,15 +3073,15 @@
         <v>17</v>
       </c>
       <c r="J19" s="35" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="29.1" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="29.15" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="C20" s="17">
         <v>1</v>
@@ -3098,15 +3105,15 @@
         <v>18</v>
       </c>
       <c r="J20" s="34" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="17">
         <v>1</v>
@@ -3130,12 +3137,12 @@
         <v>19</v>
       </c>
       <c r="J21" s="34" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>37</v>
@@ -3162,15 +3169,15 @@
         <v>20</v>
       </c>
       <c r="J22" s="34" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" s="17">
         <v>1</v>
@@ -3194,15 +3201,15 @@
         <v>21</v>
       </c>
       <c r="J23" s="35" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C24" s="17">
         <v>1</v>
@@ -3226,9 +3233,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="20" t="s">
-        <v>65</v>
+        <v>266</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="17">
@@ -3253,9 +3260,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
-        <v>65</v>
+        <v>267</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="17">
@@ -3280,7 +3287,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="20"/>
       <c r="B27" s="16" t="s">
         <v>34</v>
@@ -3295,7 +3302,7 @@
       <c r="G27" s="27"/>
       <c r="H27" s="25"/>
     </row>
-    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="12"/>
       <c r="B28" s="13"/>
       <c r="C28" s="28"/>
@@ -3319,26 +3326,26 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="44.81640625" customWidth="1"/>
+    <col min="2" max="2" width="38.81640625" customWidth="1"/>
+    <col min="3" max="3" width="7.1796875" style="31" customWidth="1"/>
     <col min="4" max="4" width="10" style="31" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="31" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="31" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="31" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" style="31" customWidth="1"/>
+    <col min="6" max="6" width="7.7265625" style="31" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>36</v>
@@ -3347,18 +3354,18 @@
         <v>33</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C2" s="36">
         <v>1</v>
@@ -3377,12 +3384,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="17">
         <v>1</v>
@@ -3403,12 +3410,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C4" s="17">
         <v>1</v>
@@ -3429,12 +3436,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C5" s="17">
         <v>1</v>
@@ -3455,12 +3462,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C6" s="17">
         <v>1</v>
@@ -3481,12 +3488,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C7" s="17">
         <v>1</v>
@@ -3507,12 +3514,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C8" s="17">
         <v>1</v>
@@ -3533,12 +3540,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C9" s="17">
         <v>1</v>
@@ -3559,12 +3566,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C10" s="17">
         <v>1</v>
@@ -3585,12 +3592,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="C11" s="17">
         <v>1</v>
@@ -3611,12 +3618,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C12" s="17">
         <v>1</v>
@@ -3637,7 +3644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="16" t="s">
         <v>34</v>
@@ -3667,156 +3674,170 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="60" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" style="72" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="60" customWidth="1"/>
-    <col min="4" max="4" width="2.85546875" style="60" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="60" customWidth="1"/>
-    <col min="6" max="8" width="13" style="60" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="60"/>
+    <col min="1" max="1" width="35.453125" style="58" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" style="62" customWidth="1"/>
+    <col min="3" max="3" width="2.81640625" style="58" customWidth="1"/>
+    <col min="4" max="4" width="23.453125" style="58" customWidth="1"/>
+    <col min="5" max="7" width="13" style="58" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="57" t="s">
-        <v>210</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="59" t="s">
-        <v>56</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="B1" s="79" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1" s="45"/>
       <c r="E1" s="45"/>
       <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="63"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="45"/>
       <c r="E2" s="45"/>
       <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="65"/>
-      <c r="H3" s="49"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="60"/>
+      <c r="G3" s="49"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="47" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="65"/>
+        <v>95</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="60"/>
+      <c r="E4" s="49"/>
       <c r="F4" s="49"/>
       <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="65"/>
+        <v>115</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="60"/>
+      <c r="E5" s="49"/>
       <c r="F5" s="49"/>
       <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="65"/>
+        <v>96</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="60"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="49"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="49"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66" t="s">
-        <v>211</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="60"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="49"/>
       <c r="F7" s="49"/>
       <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-    </row>
-    <row r="8" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="67" t="s">
-        <v>113</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="60"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
       <c r="F8" s="49"/>
       <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-    </row>
-    <row r="9" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="65"/>
+        <v>274</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="60"/>
+      <c r="D9" s="49"/>
       <c r="E9" s="49"/>
       <c r="F9" s="49"/>
       <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="69" t="s">
-        <v>121</v>
-      </c>
-      <c r="B10" s="70" t="s">
-        <v>122</v>
-      </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="65"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="81" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="60"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="49"/>
       <c r="F10" s="49"/>
       <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="74" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12" s="75"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="50" t="s">
+        <v>272</v>
+      </c>
+      <c r="B13" s="78" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="F13" s="62"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="77" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="F14" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3828,27 +3849,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="46" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" style="46" customWidth="1"/>
+    <col min="1" max="1" width="28.453125" style="46" customWidth="1"/>
+    <col min="2" max="2" width="35.7265625" style="46" customWidth="1"/>
     <col min="3" max="3" width="12" style="46" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="46"/>
+    <col min="4" max="4" width="9.1796875" style="46"/>
     <col min="5" max="5" width="13" style="46" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="46"/>
+    <col min="6" max="16384" width="9.1796875" style="46"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
@@ -3858,10 +3879,10 @@
     </row>
     <row r="2" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C2" s="25">
         <v>2</v>
@@ -3875,7 +3896,7 @@
     <row r="3" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
       <c r="B3" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C3" s="25">
         <v>2</v>
@@ -3889,39 +3910,39 @@
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="B4" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C4" s="25">
         <v>2</v>
       </c>
       <c r="D4" s="48"/>
       <c r="E4" s="50" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="51"/>
       <c r="H4" s="52"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C5" s="25">
         <v>2</v>
       </c>
       <c r="D5" s="48"/>
       <c r="E5" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" s="53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3935,16 +3956,16 @@
       </c>
       <c r="D6" s="48"/>
       <c r="E6" s="12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3960,149 +3981,149 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="80" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="73" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" style="73" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="73" customWidth="1"/>
-    <col min="5" max="7" width="10" style="74" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="73"/>
-    <col min="9" max="9" width="30.140625" style="73" customWidth="1"/>
-    <col min="10" max="11" width="44.28515625" style="73" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="73"/>
+    <col min="1" max="1" width="24.453125" style="70" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" style="63" customWidth="1"/>
+    <col min="3" max="3" width="45.81640625" style="63" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" style="63" customWidth="1"/>
+    <col min="5" max="7" width="10" style="64" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="63"/>
+    <col min="9" max="9" width="30.1796875" style="63" customWidth="1"/>
+    <col min="10" max="11" width="44.26953125" style="63" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="45" customFormat="1" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="45" customFormat="1" ht="29.15" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" s="75" t="s">
-        <v>141</v>
-      </c>
-      <c r="F1" s="75" t="s">
-        <v>140</v>
-      </c>
-      <c r="G1" s="76" t="s">
-        <v>142</v>
+        <v>135</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="66" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="49" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F2" s="56">
         <v>0</v>
       </c>
-      <c r="G2" s="77">
+      <c r="G2" s="67">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="49" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="56" t="s">
+        <v>213</v>
+      </c>
+      <c r="G3" s="67">
+        <v>0</v>
+      </c>
+      <c r="J3" s="49" t="s">
         <v>229</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="E3" s="56" t="s">
-        <v>217</v>
-      </c>
-      <c r="F3" s="56" t="s">
-        <v>218</v>
-      </c>
-      <c r="G3" s="77">
-        <v>0</v>
-      </c>
-      <c r="J3" s="49" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="49" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" s="56" t="s">
         <v>220</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="E4" s="56" t="s">
-        <v>225</v>
-      </c>
       <c r="F4" s="56">
         <v>0</v>
       </c>
-      <c r="G4" s="77">
+      <c r="G4" s="67">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="49" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F5" s="56">
         <v>0</v>
       </c>
-      <c r="G5" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="49" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E6" s="56">
         <v>0</v>
@@ -4110,45 +4131,45 @@
       <c r="F6" s="56">
         <v>0</v>
       </c>
-      <c r="G6" s="77">
+      <c r="G6" s="67">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="49" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E7" s="56" t="s">
         <v>231</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="E7" s="56" t="s">
-        <v>236</v>
-      </c>
       <c r="F7" s="56">
         <v>0</v>
       </c>
-      <c r="G7" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="E8" s="56">
         <v>0</v>
@@ -4156,45 +4177,45 @@
       <c r="F8" s="56">
         <v>0</v>
       </c>
-      <c r="G8" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="49" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="G8" s="67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="49" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F9" s="56" t="s">
-        <v>148</v>
-      </c>
-      <c r="G9" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="49" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="G9" s="67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="49" customFormat="1" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="56" t="s">
         <v>10</v>
@@ -4202,22 +4223,22 @@
       <c r="F10" s="56">
         <v>0</v>
       </c>
-      <c r="G10" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="49" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="G10" s="67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="49" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E11" s="56">
         <v>0</v>
@@ -4225,22 +4246,22 @@
       <c r="F11" s="56">
         <v>0</v>
       </c>
-      <c r="G11" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="49" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="G11" s="67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="49" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E12" s="56" t="s">
         <v>12</v>
@@ -4248,22 +4269,22 @@
       <c r="F12" s="56">
         <v>0</v>
       </c>
-      <c r="G12" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="49" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="49" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E13" s="56" t="s">
         <v>14</v>
@@ -4271,22 +4292,22 @@
       <c r="F13" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="77" t="s">
+      <c r="G13" s="67" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="49" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="49" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E14" s="56" t="s">
         <v>14</v>
@@ -4294,45 +4315,45 @@
       <c r="F14" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="77" t="s">
+      <c r="G14" s="67" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="49" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="49" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E15" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="F15" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E15" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="G15" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="49" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="G15" s="67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="49" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E16" s="56" t="s">
         <v>31</v>
@@ -4340,161 +4361,161 @@
       <c r="F16" s="56">
         <v>0</v>
       </c>
-      <c r="G16" s="77">
-        <v>0</v>
-      </c>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-    </row>
-    <row r="17" spans="1:10" s="49" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="G16" s="67">
+        <v>0</v>
+      </c>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+    </row>
+    <row r="17" spans="1:10" s="49" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" s="56">
+        <v>0</v>
+      </c>
+      <c r="F17" s="56">
+        <v>0</v>
+      </c>
+      <c r="G17" s="67">
+        <v>0</v>
+      </c>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+    </row>
+    <row r="18" spans="1:10" s="49" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="F18" s="56">
+        <v>0</v>
+      </c>
+      <c r="G18" s="67">
+        <v>0</v>
+      </c>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+    </row>
+    <row r="19" spans="1:10" s="49" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" s="56" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="G19" s="67">
+        <v>0</v>
+      </c>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+    </row>
+    <row r="20" spans="1:10" s="49" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A20" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E20" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="F20" s="56">
+        <v>0</v>
+      </c>
+      <c r="G20" s="67">
+        <v>0</v>
+      </c>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+    </row>
+    <row r="21" spans="1:10" s="49" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A21" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E21" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="56">
+        <v>0</v>
+      </c>
+      <c r="G21" s="67">
+        <v>0</v>
+      </c>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
+    </row>
+    <row r="22" spans="1:10" s="49" customFormat="1" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="E17" s="56">
-        <v>0</v>
-      </c>
-      <c r="F17" s="56">
-        <v>0</v>
-      </c>
-      <c r="G17" s="77">
-        <v>0</v>
-      </c>
-      <c r="I17" s="73"/>
-      <c r="J17" s="73"/>
-    </row>
-    <row r="18" spans="1:10" s="49" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E18" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="F18" s="56">
-        <v>0</v>
-      </c>
-      <c r="G18" s="77">
-        <v>0</v>
-      </c>
-      <c r="I18" s="73"/>
-      <c r="J18" s="73"/>
-    </row>
-    <row r="19" spans="1:10" s="49" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="E19" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="F19" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="G19" s="77">
-        <v>0</v>
-      </c>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
-    </row>
-    <row r="20" spans="1:10" s="49" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E20" s="56" t="s">
-        <v>146</v>
-      </c>
-      <c r="F20" s="56">
-        <v>0</v>
-      </c>
-      <c r="G20" s="77">
-        <v>0</v>
-      </c>
-      <c r="I20" s="73"/>
-      <c r="J20" s="73"/>
-    </row>
-    <row r="21" spans="1:10" s="49" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E21" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="56">
-        <v>0</v>
-      </c>
-      <c r="G21" s="77">
-        <v>0</v>
-      </c>
-      <c r="I21" s="73"/>
-      <c r="J21" s="73"/>
-    </row>
-    <row r="22" spans="1:10" s="49" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="E22" s="78" t="s">
-        <v>137</v>
-      </c>
-      <c r="F22" s="78">
-        <v>0</v>
-      </c>
-      <c r="G22" s="79">
-        <v>0</v>
-      </c>
-      <c r="I22" s="73"/>
-      <c r="J22" s="73"/>
+      <c r="E22" s="68" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="68">
+        <v>0</v>
+      </c>
+      <c r="G22" s="69">
+        <v>0</v>
+      </c>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4510,22 +4531,22 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.1796875" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
     <col min="3" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>36</v>
@@ -4534,21 +4555,21 @@
         <v>33</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C2" s="36">
         <v>1</v>
@@ -4564,13 +4585,13 @@
         <v>0</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H2" s="39">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="4"/>
       <c r="C3" s="17"/>
@@ -4580,7 +4601,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="25"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
       <c r="B4" s="4"/>
       <c r="C4" s="17"/>
@@ -4590,7 +4611,7 @@
       <c r="G4" s="19"/>
       <c r="H4" s="25"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="4"/>
       <c r="C5" s="17"/>
@@ -4600,7 +4621,7 @@
       <c r="G5" s="19"/>
       <c r="H5" s="25"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="4"/>
       <c r="C6" s="17"/>
@@ -4610,7 +4631,7 @@
       <c r="G6" s="19"/>
       <c r="H6" s="25"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="4"/>
       <c r="C7" s="17"/>
@@ -4634,21 +4655,21 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
+    <col min="1" max="1" width="40.81640625" customWidth="1"/>
     <col min="2" max="2" width="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>36</v>
@@ -4657,21 +4678,21 @@
         <v>33</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="C2" s="17">
         <v>1</v>
@@ -4687,18 +4708,18 @@
         <v>0</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H2" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="17">
         <v>1</v>
@@ -4715,19 +4736,19 @@
         <v>4</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H3" s="17">
         <f t="shared" ref="H3:H9" si="0">H2+1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C4" s="17">
         <v>1</v>
@@ -4750,10 +4771,10 @@
     </row>
     <row r="5" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C5" s="17">
         <v>1</v>
@@ -4769,7 +4790,7 @@
         <f t="shared" ref="F5:F9" si="2">F4+E5</f>
         <v>8</v>
       </c>
-      <c r="G5" s="81">
+      <c r="G5" s="71">
         <f>G4+1</f>
         <v>5</v>
       </c>
@@ -4780,10 +4801,10 @@
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C6" s="17">
         <v>1</v>
@@ -4799,7 +4820,7 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="G6" s="81">
+      <c r="G6" s="71">
         <f t="shared" ref="G6:G9" si="3">G5+1</f>
         <v>6</v>
       </c>
@@ -4810,10 +4831,10 @@
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C7" s="17">
         <v>1</v>
@@ -4829,7 +4850,7 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="G7" s="81">
+      <c r="G7" s="71">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
@@ -4840,10 +4861,10 @@
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C8" s="17">
         <v>1</v>
@@ -4859,7 +4880,7 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="G8" s="81">
+      <c r="G8" s="71">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
@@ -4870,10 +4891,10 @@
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C9" s="17">
         <v>1</v>
@@ -4889,7 +4910,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="G9" s="81">
+      <c r="G9" s="71">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
@@ -4898,7 +4919,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="17"/>
@@ -4922,21 +4943,21 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
+    <col min="2" max="2" width="27.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>36</v>
@@ -4945,21 +4966,21 @@
         <v>33</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C2" s="36">
         <v>1</v>
@@ -4975,18 +4996,18 @@
         <v>0</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H2" s="39">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="17">
         <v>1</v>
@@ -5003,19 +5024,19 @@
         <v>4</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H3" s="25">
         <f t="shared" ref="H3:H12" si="0">H2+1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C4" s="17">
         <v>1</v>
@@ -5041,10 +5062,10 @@
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C5" s="17">
         <v>1</v>
@@ -5070,10 +5091,10 @@
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C6" s="17">
         <v>1</v>
@@ -5099,10 +5120,10 @@
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C7" s="17">
         <v>1</v>
@@ -5128,10 +5149,10 @@
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C8" s="17">
         <v>1</v>
@@ -5157,10 +5178,10 @@
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C9" s="17">
         <v>1</v>
@@ -5186,10 +5207,10 @@
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C10" s="17">
         <v>1</v>
@@ -5215,10 +5236,10 @@
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="C11" s="17">
         <v>1</v>
@@ -5244,10 +5265,10 @@
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C12" s="17">
         <v>1</v>
@@ -5271,7 +5292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="16" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
additions to cmdAndTlm xls
</commit_message>
<xml_diff>
--- a/AVC_Docs/AVC_CmdAndTlmAndTest_v2.xlsx
+++ b/AVC_Docs/AVC_CmdAndTlmAndTest_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10380" yWindow="0" windowWidth="15360" windowHeight="11020" tabRatio="828"/>
+    <workbookView xWindow="10380" yWindow="0" windowWidth="15360" windowHeight="11020" tabRatio="828" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Rpi to Iop Cmds" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Rpi to GUI Tlm-IOP" sheetId="6" r:id="rId7"/>
     <sheet name="Rpi to GUI Tlm-Rpi" sheetId="9" r:id="rId8"/>
     <sheet name="Rpi to GUI Tlm-Diag" sheetId="10" r:id="rId9"/>
+    <sheet name="Rpi to Gui OccGrid" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'GUI to Rpi Cmds'!$A$1:$G$22</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="283">
   <si>
     <t>Notes</t>
   </si>
@@ -1014,6 +1015,28 @@
 3 - Incorrect mode
 4 - Out of limits
 5 - Unknown (should never occur)</t>
+  </si>
+  <si>
+    <t>0xDEAD</t>
+  </si>
+  <si>
+    <t>Occupancy Grid Telemetry  from Rpi to GUI
+Will be sent to GUI port xxxx.</t>
+  </si>
+  <si>
+    <t>Always 0xA5A5A5A5</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>Angle of grid result</t>
+  </si>
+  <si>
+    <t>Array of chars (300 x 50 TBD)</t>
+  </si>
+  <si>
+    <t>Occcupancy Grid</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1080,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1383,11 +1406,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1625,6 +1712,49 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1929,7 +2059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -2453,12 +2583,175 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="93" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="95" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="95" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="96" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="86"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="63"/>
+    </row>
+    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="89" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2" s="48">
+        <v>1</v>
+      </c>
+      <c r="D2" s="48">
+        <v>4</v>
+      </c>
+      <c r="E2" s="48">
+        <f>C2*D2</f>
+        <v>4</v>
+      </c>
+      <c r="F2" s="90">
+        <v>0</v>
+      </c>
+      <c r="G2" s="87"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="63"/>
+    </row>
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="89" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="48">
+        <v>1</v>
+      </c>
+      <c r="D3" s="48">
+        <v>4</v>
+      </c>
+      <c r="E3" s="48">
+        <f>C3*D3</f>
+        <v>4</v>
+      </c>
+      <c r="F3" s="90">
+        <f>F2+E3</f>
+        <v>4</v>
+      </c>
+      <c r="G3" s="87"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="63"/>
+    </row>
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="89" t="s">
+        <v>279</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>280</v>
+      </c>
+      <c r="C4" s="48">
+        <v>1</v>
+      </c>
+      <c r="D4" s="48">
+        <v>2</v>
+      </c>
+      <c r="E4" s="48">
+        <f>C4*D4</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="90">
+        <f>F3+E4</f>
+        <v>6</v>
+      </c>
+      <c r="G4" s="87"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="63"/>
+    </row>
+    <row r="5" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="76" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5" s="84" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5" s="91">
+        <v>15000</v>
+      </c>
+      <c r="D5" s="91">
+        <v>1</v>
+      </c>
+      <c r="E5" s="91">
+        <f t="shared" ref="E5:E6" si="0">C5*D5</f>
+        <v>15000</v>
+      </c>
+      <c r="F5" s="92">
+        <f t="shared" ref="F5:F6" si="1">F4+E5</f>
+        <v>15006</v>
+      </c>
+      <c r="G5" s="88"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="63"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="49"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="63"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="63"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2694,7 +2987,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="29.15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>25</v>
       </c>
@@ -2886,7 +3179,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="29.15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
         <v>40</v>
       </c>
@@ -3076,7 +3369,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="29.15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
         <v>60</v>
       </c>
@@ -3108,7 +3401,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="20" t="s">
         <v>62</v>
       </c>
@@ -3847,10 +4140,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3858,12 +4151,12 @@
     <col min="1" max="1" width="28.453125" style="46" customWidth="1"/>
     <col min="2" max="2" width="35.7265625" style="46" customWidth="1"/>
     <col min="3" max="3" width="12" style="46" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="46"/>
-    <col min="5" max="5" width="13" style="46" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="46"/>
+    <col min="4" max="5" width="9.1796875" style="46"/>
+    <col min="6" max="6" width="13" style="46" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>203</v>
       </c>
@@ -3876,8 +4169,9 @@
       <c r="F1" s="45"/>
       <c r="G1" s="45"/>
       <c r="H1" s="45"/>
-    </row>
-    <row r="2" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="I1" s="45"/>
+    </row>
+    <row r="2" spans="1:17" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A2" s="47" t="s">
         <v>103</v>
       </c>
@@ -3888,12 +4182,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="48"/>
-      <c r="E2" s="49"/>
+      <c r="E2" s="48"/>
       <c r="F2" s="49"/>
       <c r="G2" s="49"/>
       <c r="H2" s="49"/>
-    </row>
-    <row r="3" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="49"/>
+    </row>
+    <row r="3" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="20"/>
       <c r="B3" s="4" t="s">
         <v>99</v>
@@ -3902,12 +4197,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="48"/>
-      <c r="E3" s="49"/>
+      <c r="E3" s="48"/>
       <c r="F3" s="49"/>
       <c r="G3" s="49"/>
       <c r="H3" s="49"/>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I3" s="49"/>
+    </row>
+    <row r="4" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="47"/>
       <c r="B4" s="4" t="s">
         <v>100</v>
@@ -3916,14 +4212,23 @@
         <v>2</v>
       </c>
       <c r="D4" s="48"/>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="48"/>
+      <c r="F4" s="45" t="s">
         <v>204</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="52"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="82"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="20"/>
       <c r="B5" s="4" t="s">
         <v>101</v>
@@ -3932,20 +4237,47 @@
         <v>2</v>
       </c>
       <c r="D5" s="48"/>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="52" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="L5" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="P5" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" s="52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="54"/>
       <c r="B6" s="55" t="s">
         <v>34</v>
@@ -3955,17 +4287,44 @@
         <v>8</v>
       </c>
       <c r="D6" s="48"/>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="F6" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="84" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="H6" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="H6" s="14" t="s">
-        <v>101</v>
+      <c r="I6" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" s="84" t="s">
+        <v>111</v>
+      </c>
+      <c r="K6" s="77" t="s">
+        <v>112</v>
+      </c>
+      <c r="L6" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="M6" s="84" t="s">
+        <v>111</v>
+      </c>
+      <c r="N6" s="77" t="s">
+        <v>112</v>
+      </c>
+      <c r="O6" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="P6" s="84" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q6" s="77" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -4652,7 +5011,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5307,7 +5666,7 @@
       <c r="G13" s="27"/>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
       <c r="C14" s="28"/>

</xml_diff>

<commit_message>
cmd and tlm spreadsheet
</commit_message>
<xml_diff>
--- a/AVC_Docs/AVC_CmdAndTlmAndTest_v2.xlsx
+++ b/AVC_Docs/AVC_CmdAndTlmAndTest_v2.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="290">
   <si>
     <t>Notes</t>
   </si>
@@ -1024,19 +1024,40 @@
 Will be sent to GUI port xxxx.</t>
   </si>
   <si>
-    <t>Always 0xA5A5A5A5</t>
-  </si>
-  <si>
-    <t>Angle</t>
-  </si>
-  <si>
-    <t>Angle of grid result</t>
-  </si>
-  <si>
-    <t>Array of chars (300 x 50 TBD)</t>
-  </si>
-  <si>
     <t>Occcupancy Grid</t>
+  </si>
+  <si>
+    <t>Always 0x55555555</t>
+  </si>
+  <si>
+    <t>Number of Rows</t>
+  </si>
+  <si>
+    <t>Number of Cols</t>
+  </si>
+  <si>
+    <t>Car position Row</t>
+  </si>
+  <si>
+    <t>Car Position Col</t>
+  </si>
+  <si>
+    <t>Angle result</t>
+  </si>
+  <si>
+    <t>signed integer</t>
+  </si>
+  <si>
+    <t>Angle of analysis result - signed int.  Positive is CW neg is CCW</t>
+  </si>
+  <si>
+    <t>Array of bytes (300 x 50 TBD)</t>
+  </si>
+  <si>
+    <t>Checksum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summation of all integer except for the checksum itself.  </t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1101,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1433,48 +1454,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1744,16 +1728,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2585,47 +2566,47 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="23.36328125" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="73" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="93" t="s">
+    <row r="1" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="50" t="s">
         <v>277</v>
       </c>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="94" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="95" t="s">
+      <c r="D1" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="95" t="s">
+      <c r="E1" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="96" t="s">
+      <c r="F1" s="95" t="s">
         <v>180</v>
       </c>
       <c r="G1" s="86"/>
       <c r="H1" s="85"/>
       <c r="I1" s="63"/>
     </row>
-    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="89" t="s">
         <v>178</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C2" s="48">
         <v>1</v>
@@ -2644,7 +2625,7 @@
       <c r="H2" s="48"/>
       <c r="I2" s="63"/>
     </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="89" t="s">
         <v>4</v>
       </c>
@@ -2669,77 +2650,191 @@
       <c r="H3" s="48"/>
       <c r="I3" s="63"/>
     </row>
-    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="89" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="C4" s="48">
         <v>1</v>
       </c>
       <c r="D4" s="48">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E4" s="48">
-        <f>C4*D4</f>
-        <v>2</v>
+        <f t="shared" ref="E4:E10" si="0">C4*D4</f>
+        <v>4</v>
       </c>
       <c r="F4" s="90">
-        <f>F3+E4</f>
-        <v>6</v>
+        <f t="shared" ref="F4:F10" si="1">F3+E4</f>
+        <v>8</v>
       </c>
       <c r="G4" s="87"/>
       <c r="H4" s="48"/>
       <c r="I4" s="63"/>
     </row>
-    <row r="5" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="76" t="s">
-        <v>282</v>
-      </c>
-      <c r="B5" s="84" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="89" t="s">
         <v>281</v>
       </c>
-      <c r="C5" s="91">
-        <v>15000</v>
-      </c>
-      <c r="D5" s="91">
-        <v>1</v>
-      </c>
-      <c r="E5" s="91">
-        <f t="shared" ref="E5:E6" si="0">C5*D5</f>
-        <v>15000</v>
-      </c>
-      <c r="F5" s="92">
-        <f t="shared" ref="F5:F6" si="1">F4+E5</f>
-        <v>15006</v>
-      </c>
-      <c r="G5" s="88"/>
+      <c r="B5" s="49" t="s">
+        <v>285</v>
+      </c>
+      <c r="C5" s="48">
+        <v>1</v>
+      </c>
+      <c r="D5" s="48">
+        <v>4</v>
+      </c>
+      <c r="E5" s="48">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F5" s="90">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G5" s="87"/>
       <c r="H5" s="48"/>
       <c r="I5" s="63"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="49"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="88"/>
+      <c r="A6" s="89" t="s">
+        <v>282</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>285</v>
+      </c>
+      <c r="C6" s="48">
+        <v>1</v>
+      </c>
+      <c r="D6" s="48">
+        <v>4</v>
+      </c>
+      <c r="E6" s="48">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F6" s="90">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="G6" s="87"/>
       <c r="H6" s="48"/>
       <c r="I6" s="63"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="63"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
+      <c r="A7" s="89" t="s">
+        <v>283</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>285</v>
+      </c>
+      <c r="C7" s="48">
+        <v>1</v>
+      </c>
+      <c r="D7" s="48">
+        <v>4</v>
+      </c>
+      <c r="E7" s="48">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F7" s="90">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="G7" s="87"/>
+      <c r="H7" s="48"/>
       <c r="I7" s="63"/>
+    </row>
+    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="89" t="s">
+        <v>284</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="C8" s="48">
+        <v>1</v>
+      </c>
+      <c r="D8" s="48">
+        <v>4</v>
+      </c>
+      <c r="E8" s="48">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F8" s="90">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="G8" s="87"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="63"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="89" t="s">
+        <v>278</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" s="48">
+        <v>15000</v>
+      </c>
+      <c r="D9" s="48">
+        <v>1</v>
+      </c>
+      <c r="E9" s="48">
+        <f t="shared" si="0"/>
+        <v>15000</v>
+      </c>
+      <c r="F9" s="90">
+        <f t="shared" si="1"/>
+        <v>15024</v>
+      </c>
+      <c r="G9" s="88"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="63"/>
+    </row>
+    <row r="10" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="76" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" s="84" t="s">
+        <v>289</v>
+      </c>
+      <c r="C10" s="91">
+        <v>1</v>
+      </c>
+      <c r="D10" s="91">
+        <v>4</v>
+      </c>
+      <c r="E10" s="91">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F10" s="92">
+        <f t="shared" si="1"/>
+        <v>15028</v>
+      </c>
+      <c r="G10" s="88"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="63"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="63"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>